<commit_message>
Changed color of cell
in yellow
</commit_message>
<xml_diff>
--- a/XC60 vs V70.xlsx
+++ b/XC60 vs V70.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_e5c\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0d9f4414b6a1f8e/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="11_924858E5C0DEB8026F15A6DB943E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{34026B4E-A347-4CAF-AEA9-0732C68BDA4E}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="11_924858E5C0DEB8026F15A6DB943E8C1851038383" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{32D3D93C-8734-FB42-B21B-16E2BE9B4B47}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="57600" windowHeight="31940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -144,12 +144,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -173,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -194,9 +200,10 @@
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -237,7 +244,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -535,21 +542,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="60.28515625" customWidth="1"/>
+    <col min="5" max="5" width="60.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -565,7 +570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -582,7 +587,7 @@
         <v>-844</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -602,7 +607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -617,7 +622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -629,7 +634,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -644,7 +649,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -662,7 +667,7 @@
       </c>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -674,7 +679,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
@@ -686,7 +691,7 @@
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
@@ -698,7 +703,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -710,28 +715,28 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D12" s="13">
         <f>D2+D3+D7</f>
         <v>-592.40097870316617</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
     </row>
-    <row r="17" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
     </row>
-    <row r="18" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
     </row>
-    <row r="19" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
     </row>
-    <row r="20" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change formula for total diff
</commit_message>
<xml_diff>
--- a/XC60 vs V70.xlsx
+++ b/XC60 vs V70.xlsx
@@ -8,22 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0d9f4414b6a1f8e/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="11_924858E5C0DEB8026F15A6DB943E8C1851038383" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{32D3D93C-8734-FB42-B21B-16E2BE9B4B47}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="11_924858E5C0DEB8026F15A6DB943E8C1851038383" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{D5BFB73E-AAC1-ED42-8AD4-A868D6239D67}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="57600" windowHeight="31940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -112,7 +104,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+  <numFmts count="9">
+    <numFmt numFmtId="44" formatCode="_(&quot;€&quot;\ * #,##0.00_);_(&quot;€&quot;\ * \(#,##0.00\);_(&quot;€&quot;\ * &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ [$€-2]\ * #,##0_ ;_ [$€-2]\ * \-#,##0_ ;_ [$€-2]\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="0.0"/>
@@ -120,9 +113,9 @@
     <numFmt numFmtId="168" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="170" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="171" formatCode="_ [$€-2]\ * #,##0.0000_ ;_ [$€-2]\ * \-#,##0.0000_ ;_ [$€-2]\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="172" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +135,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -176,8 +176,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -197,17 +198,18 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Valuta" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="171" formatCode="_ [$€-2]\ * #,##0.0000_ ;_ [$€-2]\ * \-#,##0.0000_ ;_ [$€-2]\ * &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="172" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -233,9 +235,9 @@
     <tableColumn id="1" xr3:uid="{2EFAE5B8-0483-4BDC-B5E9-A573A5854B58}" name="Kolom1"/>
     <tableColumn id="2" xr3:uid="{0B94F273-FF4C-475C-B1AE-F5CF382D7586}" name="XC60"/>
     <tableColumn id="3" xr3:uid="{88600520-EDAE-4C58-A24B-EF13B8F1D20B}" name="V70"/>
-    <tableColumn id="5" xr3:uid="{77C94949-0EDC-4C63-8766-2DB042963F35}" name="Verschil" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
+    <tableColumn id="5" xr3:uid="{77C94949-0EDC-4C63-8766-2DB042963F35}" name="Verschil" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0" totalsRowCellStyle="Valuta">
       <calculatedColumnFormula>B2-C2</calculatedColumnFormula>
-      <totalsRowFormula>D2+D3+D7</totalsRowFormula>
+      <totalsRowFormula>SUM(D2:D11)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{C7F4534B-927A-4F28-B9EC-DF72A6E39A5B}" name="Toelichting"/>
   </tableColumns>
@@ -542,7 +544,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -554,7 +558,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -716,8 +720,8 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="13">
-        <f>D2+D3+D7</f>
+      <c r="D12" s="14">
+        <f>SUM(D2:D11)</f>
         <v>-592.40097870316617</v>
       </c>
     </row>

</xml_diff>